<commit_message>
added total volumes needed
</commit_message>
<xml_diff>
--- a/metadata/Virginica-MBDSeq-Labwork-Calculations.xlsx
+++ b/metadata/Virginica-MBDSeq-Labwork-Calculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-cv-cg-trans-meth/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-oyster-comparative-omics/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEB10FE-A7FE-8D4B-99BA-DF15C99D523F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E70726-2281-2745-867C-F6267FD049A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="32000" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sperm" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Sample</t>
   </si>
@@ -92,12 +92,6 @@
     <t>Volume for 25 ng/µL concentration (µL)</t>
   </si>
   <si>
-    <t>New concentration (ng/µL)</t>
-  </si>
-  <si>
-    <t>Volume water needed to dilute to 25 ng/µL (µL)</t>
-  </si>
-  <si>
     <t>Volume water needed</t>
   </si>
   <si>
@@ -137,7 +131,10 @@
     <t>L18A0063s</t>
   </si>
   <si>
-    <t>L18A0031s Volume after speed vacuum (µL)</t>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Treatment</t>
   </si>
 </sst>
 </file>
@@ -187,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -202,6 +199,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,991 +483,1034 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="153">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="153">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
       <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2">
         <v>96</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>44</v>
       </c>
-      <c r="D2">
-        <f>B2*C2</f>
+      <c r="E2">
+        <f>C2*D2</f>
         <v>4224</v>
       </c>
-      <c r="E2">
-        <f>0.001*D2</f>
+      <c r="F2">
+        <f>0.001*E2</f>
         <v>4.2240000000000002</v>
       </c>
-      <c r="F2">
-        <f>(B2*C2)/25</f>
+      <c r="G2">
+        <f>(C2*D2)/25</f>
         <v>168.96</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>4</v>
       </c>
-      <c r="H2">
-        <f>(G2*F2)/E2</f>
+      <c r="I2">
+        <f>(H2*G2)/F2</f>
         <v>160</v>
       </c>
-      <c r="I2">
-        <f>G2*10</f>
+      <c r="J2">
+        <f>H2*10</f>
         <v>40</v>
       </c>
-      <c r="J2">
-        <f>G2*7</f>
+      <c r="K2">
+        <f>H2*7</f>
         <v>28</v>
       </c>
-      <c r="K2">
-        <f>100-I2</f>
+      <c r="L2">
+        <f>100-J2</f>
         <v>60</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="M2">
-        <f>K2+2*L2</f>
+      <c r="N2">
+        <f>L2+2*M2</f>
         <v>260</v>
       </c>
-      <c r="N2">
-        <f>200-J2</f>
+      <c r="O2">
+        <f>200-K2</f>
         <v>172</v>
       </c>
-      <c r="O2">
-        <f>L2</f>
-        <v>100</v>
-      </c>
       <c r="P2">
-        <f>3*O2</f>
+        <f>M2</f>
+        <v>100</v>
+      </c>
+      <c r="Q2">
+        <f>3*P2</f>
         <v>300</v>
       </c>
-      <c r="Q2">
-        <f>O2</f>
-        <v>100</v>
-      </c>
       <c r="R2">
-        <f>SUM(M2,N2,P2,Q2)</f>
+        <f>P2</f>
+        <v>100</v>
+      </c>
+      <c r="S2">
+        <f>SUM(N2,O2,Q2,R2)</f>
         <v>832</v>
       </c>
-      <c r="S2">
-        <f>500-100-H2</f>
+      <c r="T2">
+        <f>500-100-I2</f>
         <v>240</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <f>200*4</f>
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
         <v>432</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>43</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D12" si="0">B3*C3</f>
+      <c r="E3">
+        <f t="shared" ref="E3:E12" si="0">C3*D3</f>
         <v>18576</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E12" si="1">0.001*D3</f>
+      <c r="F3">
+        <f t="shared" ref="F3:F12" si="1">0.001*E3</f>
         <v>18.576000000000001</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F12" si="2">(B3*C3)/25</f>
+      <c r="G3">
+        <f t="shared" ref="G3:G12" si="2">(C3*D3)/25</f>
         <v>743.04</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>4</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H12" si="3">(G3*F3)/E3</f>
+      <c r="I3">
+        <f t="shared" ref="I3:I12" si="3">(H3*G3)/F3</f>
         <v>160</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I12" si="4">G3*10</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J12" si="4">H3*10</f>
         <v>40</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J12" si="5">G3*7</f>
+      <c r="K3">
+        <f t="shared" ref="K3:K12" si="5">H3*7</f>
         <v>28</v>
       </c>
-      <c r="K3">
-        <f>100-I3</f>
+      <c r="L3">
+        <f>100-J3</f>
         <v>60</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M12" si="6">K3+2*L3</f>
+      <c r="N3">
+        <f t="shared" ref="N3:N12" si="6">L3+2*M3</f>
         <v>260</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N12" si="7">200-J3</f>
+      <c r="O3">
+        <f t="shared" ref="O3:O12" si="7">200-K3</f>
         <v>172</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O11" si="8">L3</f>
-        <v>100</v>
-      </c>
       <c r="P3">
-        <f t="shared" ref="P3:P11" si="9">3*O3</f>
+        <f t="shared" ref="P3:P11" si="8">M3</f>
+        <v>100</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q11" si="9">3*P3</f>
         <v>300</v>
       </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q11" si="10">O3</f>
-        <v>100</v>
-      </c>
       <c r="R3">
-        <f t="shared" ref="R3:R12" si="11">SUM(M3,N3,P3,Q3)</f>
+        <f t="shared" ref="R3:R11" si="10">P3</f>
+        <v>100</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S12" si="11">SUM(N3,O3,Q3,R3)</f>
         <v>832</v>
       </c>
-      <c r="S3">
-        <f t="shared" ref="S3:S12" si="12">500-100-H3</f>
+      <c r="T3">
+        <f t="shared" ref="T3:T12" si="12">500-100-I3</f>
         <v>240</v>
       </c>
-      <c r="T3">
-        <f t="shared" ref="T3:T12" si="13">200*4</f>
+      <c r="U3">
+        <f t="shared" ref="U3:U12" si="13">200*4</f>
         <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4">
+        <v>2800</v>
+      </c>
+      <c r="C4">
         <v>46.4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>44</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>2041.6</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <f t="shared" si="1"/>
         <v>2.0415999999999999</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f t="shared" si="2"/>
         <v>81.664000000000001</v>
       </c>
-      <c r="G4">
-        <f>E4</f>
+      <c r="H4">
+        <f>F4</f>
         <v>2.0415999999999999</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <f t="shared" si="3"/>
         <v>81.664000000000001</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f t="shared" si="4"/>
         <v>20.415999999999997</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f t="shared" si="5"/>
         <v>14.2912</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <f t="shared" si="6"/>
         <v>200</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <f t="shared" si="7"/>
         <v>185.7088</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <f t="shared" si="9"/>
         <v>300</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <f t="shared" si="11"/>
         <v>785.7088</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <f t="shared" si="12"/>
         <v>318.33600000000001</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5">
+        <v>2800</v>
+      </c>
+      <c r="C5">
         <v>73.599999999999994</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>44</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>3238.3999999999996</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f t="shared" si="1"/>
         <v>3.2383999999999995</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="2"/>
         <v>129.53599999999997</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="K5">
-        <f>100-I5</f>
+      <c r="L5">
+        <f>100-J5</f>
         <v>60</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <f t="shared" si="6"/>
         <v>260</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <f t="shared" si="7"/>
         <v>172</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <f t="shared" si="9"/>
         <v>300</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <f t="shared" si="11"/>
         <v>832</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <f t="shared" si="12"/>
         <v>240</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6">
+        <v>500</v>
+      </c>
+      <c r="C6">
         <v>186</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>44</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>8184</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <f t="shared" si="1"/>
         <v>8.1840000000000011</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f t="shared" si="2"/>
         <v>327.36</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>4</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="K6">
-        <f>100-I6</f>
+      <c r="L6">
+        <f>100-J6</f>
         <v>60</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <f t="shared" si="6"/>
         <v>260</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <f t="shared" si="7"/>
         <v>172</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <f t="shared" si="9"/>
         <v>300</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <f t="shared" si="11"/>
         <v>832</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <f t="shared" si="12"/>
         <v>240</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7">
+        <v>2800</v>
+      </c>
+      <c r="C7">
         <v>344</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>43</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>14792</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f t="shared" si="1"/>
         <v>14.792</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f t="shared" si="2"/>
         <v>591.67999999999995</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f t="shared" si="6"/>
         <v>200</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <f t="shared" si="7"/>
         <v>172</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <f t="shared" si="9"/>
         <v>300</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <f t="shared" si="11"/>
         <v>772</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <f t="shared" si="12"/>
         <v>240</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2800</v>
+      </c>
+      <c r="C8">
         <v>9.24</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>44</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>406.56</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <f t="shared" si="1"/>
         <v>0.40656000000000003</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="2"/>
         <v>16.2624</v>
       </c>
-      <c r="G8">
-        <f>E8</f>
+      <c r="H8">
+        <f>F8</f>
         <v>0.40656000000000003</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f t="shared" si="3"/>
         <v>16.2624</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f t="shared" si="4"/>
         <v>4.0655999999999999</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f t="shared" si="5"/>
         <v>2.8459200000000004</v>
       </c>
-      <c r="K8">
-        <f>100-I8</f>
+      <c r="L8">
+        <f>100-J8</f>
         <v>95.934399999999997</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <f t="shared" si="6"/>
         <v>295.93439999999998</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <f t="shared" si="7"/>
         <v>197.15407999999999</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <f t="shared" si="9"/>
         <v>300</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <f t="shared" si="11"/>
         <v>893.08848</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <f t="shared" si="12"/>
         <v>383.73759999999999</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9">
+        <v>27</v>
+      </c>
+      <c r="B9" s="4">
+        <v>2800</v>
+      </c>
+      <c r="C9">
         <v>25.8</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>43</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>1109.4000000000001</v>
       </c>
-      <c r="E9">
-        <f>0.001*D9</f>
+      <c r="F9">
+        <f>0.001*E9</f>
         <v>1.1094000000000002</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f t="shared" si="2"/>
         <v>44.376000000000005</v>
       </c>
-      <c r="G9">
-        <f>E9</f>
+      <c r="H9">
+        <f>F9</f>
         <v>1.1094000000000002</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f t="shared" si="3"/>
         <v>44.376000000000005</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="4"/>
         <v>11.094000000000001</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f t="shared" si="5"/>
         <v>7.7658000000000014</v>
       </c>
-      <c r="K9">
-        <f t="shared" ref="K9:K12" si="14">100-I9</f>
+      <c r="L9">
+        <f t="shared" ref="L9:L12" si="14">100-J9</f>
         <v>88.906000000000006</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <f t="shared" si="6"/>
         <v>288.90600000000001</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <f t="shared" si="7"/>
         <v>192.23419999999999</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <f t="shared" si="9"/>
         <v>300</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <f t="shared" si="11"/>
         <v>881.14020000000005</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <f t="shared" si="12"/>
         <v>355.62400000000002</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10">
+        <v>500</v>
+      </c>
+      <c r="C10">
         <v>163</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>44</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>7172</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <f t="shared" si="1"/>
         <v>7.1719999999999997</v>
       </c>
-      <c r="F10">
-        <f>(F17*F16)/25</f>
-        <v>286.88</v>
-      </c>
       <c r="G10">
+        <f>(G17*G16)/25</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>4</v>
       </c>
-      <c r="H10">
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="14"/>
+        <v>60</v>
+      </c>
+      <c r="M10">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="6"/>
+        <v>260</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="7"/>
+        <v>172</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="11"/>
+        <v>832</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="12"/>
+        <v>400</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="13"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>2800</v>
+      </c>
+      <c r="C11">
+        <v>55.6</v>
+      </c>
+      <c r="D11">
+        <v>44</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2446.4</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>2.4464000000000001</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>97.856000000000009</v>
+      </c>
+      <c r="H11">
+        <f>F11</f>
+        <v>2.4464000000000001</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>97.856000000000009</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>24.464000000000002</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="5"/>
+        <v>17.1248</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="14"/>
+        <v>75.536000000000001</v>
+      </c>
+      <c r="M11">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="6"/>
+        <v>275.536</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="7"/>
+        <v>182.87520000000001</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="11"/>
+        <v>858.41120000000001</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="12"/>
+        <v>302.14400000000001</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="13"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>2800</v>
+      </c>
+      <c r="C12">
+        <v>99.4</v>
+      </c>
+      <c r="D12">
+        <v>44</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>4373.6000000000004</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>4.3736000000000006</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>174.94400000000002</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="I10">
+      <c r="J12">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="J10">
+      <c r="K12">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="K10">
+      <c r="L12">
         <f t="shared" si="14"/>
         <v>60</v>
       </c>
-      <c r="L10">
+      <c r="M12">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="M10">
+      <c r="N12">
         <f t="shared" si="6"/>
         <v>260</v>
       </c>
-      <c r="N10">
+      <c r="O12">
         <f t="shared" si="7"/>
         <v>172</v>
       </c>
-      <c r="O10">
-        <f t="shared" si="8"/>
-        <v>100</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="9"/>
+      <c r="P12">
+        <f t="shared" ref="P12" si="15">M12</f>
+        <v>100</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ref="Q12" si="16">3*P12</f>
         <v>300</v>
       </c>
-      <c r="Q10">
-        <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="R10">
+      <c r="R12">
+        <f t="shared" ref="R12" si="17">P12</f>
+        <v>100</v>
+      </c>
+      <c r="S12">
         <f t="shared" si="11"/>
         <v>832</v>
       </c>
-      <c r="S10">
+      <c r="T12">
         <f t="shared" si="12"/>
         <v>240</v>
       </c>
-      <c r="T10">
+      <c r="U12">
         <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
-      <c r="A11" t="s">
+    <row r="13" spans="1:21">
+      <c r="A13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B11">
-        <v>55.6</v>
-      </c>
-      <c r="C11">
-        <v>44</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>2446.4</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>2.4464000000000001</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>97.856000000000009</v>
-      </c>
-      <c r="G11">
-        <f>E11</f>
-        <v>2.4464000000000001</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="3"/>
-        <v>97.856000000000009</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="4"/>
-        <v>24.464000000000002</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="5"/>
-        <v>17.1248</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="14"/>
-        <v>75.536000000000001</v>
-      </c>
-      <c r="L11">
-        <f>100</f>
-        <v>100</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="6"/>
-        <v>275.536</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="7"/>
-        <v>182.87520000000001</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="8"/>
-        <v>100</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="9"/>
-        <v>300</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="11"/>
-        <v>858.41120000000001</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="12"/>
-        <v>302.14400000000001</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="13"/>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12">
-        <v>99.4</v>
-      </c>
-      <c r="C12">
-        <v>44</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>4373.6000000000004</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>4.3736000000000006</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>174.94400000000002</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="3"/>
-        <v>160</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="5"/>
-        <v>28</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="14"/>
-        <v>60</v>
-      </c>
-      <c r="L12">
-        <f>100</f>
-        <v>100</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="6"/>
-        <v>260</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="7"/>
-        <v>172</v>
-      </c>
-      <c r="O12">
-        <f t="shared" ref="O12" si="15">L12</f>
-        <v>100</v>
-      </c>
-      <c r="P12">
-        <f t="shared" ref="P12" si="16">3*O12</f>
-        <v>300</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" ref="Q12" si="17">O12</f>
-        <v>100</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="11"/>
-        <v>832</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="12"/>
-        <v>240</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="13"/>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="R13">
-        <f>SUM(R2:R12)</f>
+      <c r="B13" s="6"/>
+      <c r="J13">
+        <f>SUM(J2:J12)</f>
+        <v>340.03960000000001</v>
+      </c>
+      <c r="K13">
+        <f>SUM(K2:K12)</f>
+        <v>238.02772000000002</v>
+      </c>
+      <c r="S13">
+        <f>SUM(S2:S12)</f>
         <v>9182.348680000001</v>
       </c>
-      <c r="T13">
-        <f>SUM(T2:T12)</f>
+      <c r="U13">
+        <f>SUM(U2:U12)</f>
         <v>8800</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
-      <c r="R14">
-        <f>R13*0.001</f>
+    <row r="14" spans="1:21">
+      <c r="S14">
+        <f>S13*0.001</f>
         <v>9.1823486800000005</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="68">
-      <c r="E16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6" ht="51">
-      <c r="E17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17">
-        <f>(B10*C10)/18</f>
-        <v>398.44444444444446</v>
-      </c>
-    </row>
-    <row r="18" spans="5:6" ht="68">
-      <c r="E18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18">
-        <f>F10-F16</f>
-        <v>268.88</v>
-      </c>
+    <row r="15" spans="1:21">
+      <c r="U15">
+        <f>SUM(U13,S13)</f>
+        <v>17982.348680000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="F16" s="3"/>
+      <c r="U16">
+        <f>U15/1000</f>
+        <v>17.982348680000001</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="6:6">
+      <c r="F18" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="94" fitToWidth="2" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="K4 K7 F10" formula="1"/>
+    <ignoredError sqref="L4 L7 G10" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added a column for dilution information
</commit_message>
<xml_diff>
--- a/metadata/Virginica-MBDSeq-Labwork-Calculations.xlsx
+++ b/metadata/Virginica-MBDSeq-Labwork-Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-oyster-comparative-omics/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E70726-2281-2745-867C-F6267FD049A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8520CEAC-8EF3-1E44-A4AE-F1117479743F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="32000" windowHeight="23540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Sample</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Treatment</t>
+  </si>
+  <si>
+    <t>Volume E.Z.N.A. Buffer Needed for Dilution (µL)</t>
   </si>
 </sst>
 </file>
@@ -483,22 +486,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="153">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="153">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,49 +524,52 @@
         <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -571,80 +577,84 @@
         <v>500</v>
       </c>
       <c r="C2">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="D2">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E2">
         <f>C2*D2</f>
-        <v>4224</v>
+        <v>4840</v>
       </c>
       <c r="F2">
         <f>0.001*E2</f>
-        <v>4.2240000000000002</v>
+        <v>4.84</v>
       </c>
       <c r="G2">
         <f>(C2*D2)/25</f>
-        <v>168.96</v>
+        <v>193.6</v>
       </c>
       <c r="H2">
+        <f>G2-D2</f>
+        <v>153.6</v>
+      </c>
+      <c r="I2">
         <v>4</v>
       </c>
-      <c r="I2">
-        <f>(H2*G2)/F2</f>
+      <c r="J2">
+        <f>(I2*G2)/F2</f>
         <v>160</v>
       </c>
-      <c r="J2">
-        <f>H2*10</f>
+      <c r="K2">
+        <f>I2*10</f>
         <v>40</v>
       </c>
-      <c r="K2">
-        <f>H2*7</f>
+      <c r="L2">
+        <f>I2*7</f>
         <v>28</v>
       </c>
-      <c r="L2">
-        <f>100-J2</f>
+      <c r="M2">
+        <f>100-K2</f>
         <v>60</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="N2">
-        <f>L2+2*M2</f>
+      <c r="O2">
+        <f>M2+2*N2</f>
         <v>260</v>
       </c>
-      <c r="O2">
-        <f>200-K2</f>
+      <c r="P2">
+        <f>200-L2</f>
         <v>172</v>
       </c>
-      <c r="P2">
-        <f>M2</f>
-        <v>100</v>
-      </c>
       <c r="Q2">
-        <f>3*P2</f>
+        <f>N2</f>
+        <v>100</v>
+      </c>
+      <c r="R2">
+        <f>3*Q2</f>
         <v>300</v>
       </c>
-      <c r="R2">
-        <f>P2</f>
-        <v>100</v>
-      </c>
       <c r="S2">
-        <f>SUM(N2,O2,Q2,R2)</f>
+        <f>Q2</f>
+        <v>100</v>
+      </c>
+      <c r="T2">
+        <f>SUM(O2,P2,R2,S2)</f>
         <v>832</v>
       </c>
-      <c r="T2">
-        <f>500-100-I2</f>
+      <c r="U2">
+        <f>500-100-J2</f>
         <v>240</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <f>200*4</f>
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -652,80 +662,84 @@
         <v>500</v>
       </c>
       <c r="C3">
-        <v>432</v>
+        <v>550</v>
       </c>
       <c r="D3">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E12" si="0">C3*D3</f>
-        <v>18576</v>
+        <v>22000</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F12" si="1">0.001*E3</f>
-        <v>18.576000000000001</v>
+        <v>22</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G12" si="2">(C3*D3)/25</f>
-        <v>743.04</v>
+        <v>880</v>
       </c>
       <c r="H3">
+        <f t="shared" ref="H3:H12" si="3">G3-D3</f>
+        <v>840</v>
+      </c>
+      <c r="I3">
         <v>4</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I12" si="3">(H3*G3)/F3</f>
+      <c r="J3">
+        <f>(I3*G3)/F3</f>
         <v>160</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J12" si="4">H3*10</f>
+      <c r="K3">
+        <f>I3*10</f>
         <v>40</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K12" si="5">H3*7</f>
+      <c r="L3">
+        <f>I3*7</f>
         <v>28</v>
       </c>
-      <c r="L3">
-        <f>100-J3</f>
+      <c r="M3">
+        <f>100-K3</f>
         <v>60</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N12" si="6">L3+2*M3</f>
+      <c r="O3">
+        <f t="shared" ref="O3:O12" si="4">M3+2*N3</f>
         <v>260</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O12" si="7">200-K3</f>
+      <c r="P3">
+        <f t="shared" ref="P3:P12" si="5">200-L3</f>
         <v>172</v>
       </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P11" si="8">M3</f>
-        <v>100</v>
-      </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q11" si="9">3*P3</f>
+        <f t="shared" ref="Q3:Q11" si="6">N3</f>
+        <v>100</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R11" si="7">3*Q3</f>
         <v>300</v>
       </c>
-      <c r="R3">
-        <f t="shared" ref="R3:R11" si="10">P3</f>
-        <v>100</v>
-      </c>
       <c r="S3">
-        <f t="shared" ref="S3:S12" si="11">SUM(N3,O3,Q3,R3)</f>
+        <f t="shared" ref="S3:S11" si="8">Q3</f>
+        <v>100</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T12" si="9">SUM(O3,P3,R3,S3)</f>
         <v>832</v>
       </c>
-      <c r="T3">
-        <f t="shared" ref="T3:T12" si="12">500-100-I3</f>
+      <c r="U3">
+        <f>500-100-J3</f>
         <v>240</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U12" si="13">200*4</f>
+      <c r="V3">
+        <f t="shared" ref="V3:V12" si="10">200*4</f>
         <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -733,81 +747,84 @@
         <v>2800</v>
       </c>
       <c r="C4">
-        <v>46.4</v>
+        <v>95</v>
       </c>
       <c r="D4">
         <v>44</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>2041.6</v>
+        <v>4180</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>2.0415999999999999</v>
+        <v>4.18</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>81.664000000000001</v>
+        <v>167.2</v>
       </c>
       <c r="H4">
-        <f>F4</f>
-        <v>2.0415999999999999</v>
+        <f t="shared" si="3"/>
+        <v>123.19999999999999</v>
       </c>
       <c r="I4">
-        <f t="shared" si="3"/>
-        <v>81.664000000000001</v>
+        <v>4</v>
       </c>
       <c r="J4">
-        <f t="shared" si="4"/>
-        <v>20.415999999999997</v>
+        <f>(I4*G4)/F4</f>
+        <v>160</v>
       </c>
       <c r="K4">
-        <f t="shared" si="5"/>
-        <v>14.2912</v>
+        <f>I4*10</f>
+        <v>40</v>
       </c>
       <c r="L4">
+        <f>I4*7</f>
+        <v>28</v>
+      </c>
+      <c r="M4">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="N4">
+      <c r="O4">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="5"/>
+        <v>172</v>
+      </c>
+      <c r="Q4">
         <f t="shared" si="6"/>
-        <v>200</v>
-      </c>
-      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="R4">
         <f t="shared" si="7"/>
-        <v>185.7088</v>
-      </c>
-      <c r="P4">
+        <v>300</v>
+      </c>
+      <c r="S4">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="Q4">
+      <c r="T4">
         <f t="shared" si="9"/>
-        <v>300</v>
-      </c>
-      <c r="R4">
+        <v>772</v>
+      </c>
+      <c r="U4">
+        <f>500-100-J4</f>
+        <v>240</v>
+      </c>
+      <c r="V4">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="S4">
-        <f t="shared" si="11"/>
-        <v>785.7088</v>
-      </c>
-      <c r="T4">
-        <f t="shared" si="12"/>
-        <v>318.33600000000001</v>
-      </c>
-      <c r="U4">
-        <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -815,80 +832,84 @@
         <v>2800</v>
       </c>
       <c r="C5">
-        <v>73.599999999999994</v>
+        <v>111</v>
       </c>
       <c r="D5">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>3238.3999999999996</v>
+        <v>4440</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>3.2383999999999995</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>129.53599999999997</v>
+        <v>177.6</v>
       </c>
       <c r="H5">
+        <f t="shared" si="3"/>
+        <v>137.6</v>
+      </c>
+      <c r="I5">
         <v>4</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="3"/>
-        <v>160</v>
-      </c>
       <c r="J5">
+        <f>(I5*G5)/F5</f>
+        <v>159.99999999999997</v>
+      </c>
+      <c r="K5">
+        <f>I5*10</f>
+        <v>40</v>
+      </c>
+      <c r="L5">
+        <f>I5*7</f>
+        <v>28</v>
+      </c>
+      <c r="M5">
+        <f>100-K5</f>
+        <v>60</v>
+      </c>
+      <c r="N5">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="K5">
+        <v>260</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="5"/>
-        <v>28</v>
-      </c>
-      <c r="L5">
-        <f>100-J5</f>
-        <v>60</v>
-      </c>
-      <c r="M5">
-        <f>100</f>
-        <v>100</v>
-      </c>
-      <c r="N5">
+        <v>172</v>
+      </c>
+      <c r="Q5">
         <f t="shared" si="6"/>
-        <v>260</v>
-      </c>
-      <c r="O5">
+        <v>100</v>
+      </c>
+      <c r="R5">
         <f t="shared" si="7"/>
-        <v>172</v>
-      </c>
-      <c r="P5">
+        <v>300</v>
+      </c>
+      <c r="S5">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="Q5">
+      <c r="T5">
         <f t="shared" si="9"/>
-        <v>300</v>
-      </c>
-      <c r="R5">
+        <v>832</v>
+      </c>
+      <c r="U5">
+        <f>500-100-J5</f>
+        <v>240.00000000000003</v>
+      </c>
+      <c r="V5">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="S5">
-        <f t="shared" si="11"/>
-        <v>832</v>
-      </c>
-      <c r="T5">
-        <f t="shared" si="12"/>
-        <v>240</v>
-      </c>
-      <c r="U5">
-        <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -896,80 +917,84 @@
         <v>500</v>
       </c>
       <c r="C6">
-        <v>186</v>
+        <v>958</v>
       </c>
       <c r="D6">
         <v>44</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>8184</v>
+        <v>42152</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>8.1840000000000011</v>
+        <v>42.152000000000001</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>327.36</v>
+        <v>1686.08</v>
       </c>
       <c r="H6">
+        <f t="shared" si="3"/>
+        <v>1642.08</v>
+      </c>
+      <c r="I6">
         <v>4</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="3"/>
+      <c r="J6">
+        <f>(I6*G6)/F6</f>
         <v>160</v>
       </c>
-      <c r="J6">
+      <c r="K6">
+        <f>I6*10</f>
+        <v>40</v>
+      </c>
+      <c r="L6">
+        <f>I6*7</f>
+        <v>28</v>
+      </c>
+      <c r="M6">
+        <f>100-K6</f>
+        <v>60</v>
+      </c>
+      <c r="N6">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="K6">
+        <v>260</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="5"/>
-        <v>28</v>
-      </c>
-      <c r="L6">
-        <f>100-J6</f>
-        <v>60</v>
-      </c>
-      <c r="M6">
-        <f>100</f>
-        <v>100</v>
-      </c>
-      <c r="N6">
+        <v>172</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="6"/>
-        <v>260</v>
-      </c>
-      <c r="O6">
+        <v>100</v>
+      </c>
+      <c r="R6">
         <f t="shared" si="7"/>
-        <v>172</v>
-      </c>
-      <c r="P6">
+        <v>300</v>
+      </c>
+      <c r="S6">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="Q6">
+      <c r="T6">
         <f t="shared" si="9"/>
-        <v>300</v>
-      </c>
-      <c r="R6">
+        <v>832</v>
+      </c>
+      <c r="U6">
+        <f>500-100-J6</f>
+        <v>240</v>
+      </c>
+      <c r="V6">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="S6">
-        <f t="shared" si="11"/>
-        <v>832</v>
-      </c>
-      <c r="T6">
-        <f t="shared" si="12"/>
-        <v>240</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -977,80 +1002,84 @@
         <v>2800</v>
       </c>
       <c r="C7">
-        <v>344</v>
+        <v>318</v>
       </c>
       <c r="D7">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>14792</v>
+        <v>12720</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>14.792</v>
+        <v>12.72</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>591.67999999999995</v>
+        <v>508.8</v>
       </c>
       <c r="H7">
+        <f t="shared" si="3"/>
+        <v>468.8</v>
+      </c>
+      <c r="I7">
         <v>4</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="3"/>
+      <c r="J7">
+        <f>(I7*G7)/F7</f>
         <v>160</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="4"/>
+      <c r="K7">
+        <f>I7*10</f>
         <v>40</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="5"/>
+      <c r="L7">
+        <f>I7*7</f>
         <v>28</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="N7">
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="5"/>
+        <v>172</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="6"/>
-        <v>200</v>
-      </c>
-      <c r="O7">
+        <v>100</v>
+      </c>
+      <c r="R7">
         <f t="shared" si="7"/>
-        <v>172</v>
-      </c>
-      <c r="P7">
+        <v>300</v>
+      </c>
+      <c r="S7">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="Q7">
+      <c r="T7">
         <f t="shared" si="9"/>
-        <v>300</v>
-      </c>
-      <c r="R7">
+        <v>772</v>
+      </c>
+      <c r="U7">
+        <f>500-100-J7</f>
+        <v>240</v>
+      </c>
+      <c r="V7">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="11"/>
-        <v>772</v>
-      </c>
-      <c r="T7">
-        <f t="shared" si="12"/>
-        <v>240</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:22">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -1058,81 +1087,85 @@
         <v>2800</v>
       </c>
       <c r="C8">
-        <v>9.24</v>
+        <v>9.82</v>
       </c>
       <c r="D8">
         <v>44</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>406.56</v>
+        <v>432.08000000000004</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>0.40656000000000003</v>
+        <v>0.43208000000000008</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>16.2624</v>
+        <v>17.283200000000001</v>
       </c>
       <c r="H8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
         <f>F8</f>
-        <v>0.40656000000000003</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="3"/>
-        <v>16.2624</v>
+        <v>0.43208000000000008</v>
       </c>
       <c r="J8">
+        <f>(I8*G8)/F8</f>
+        <v>17.283200000000001</v>
+      </c>
+      <c r="K8">
+        <f>I8*10</f>
+        <v>4.3208000000000011</v>
+      </c>
+      <c r="L8">
+        <f>I8*7</f>
+        <v>3.0245600000000006</v>
+      </c>
+      <c r="M8">
+        <f>100-K8</f>
+        <v>95.679199999999994</v>
+      </c>
+      <c r="N8">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="4"/>
-        <v>4.0655999999999999</v>
-      </c>
-      <c r="K8">
+        <v>295.67919999999998</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="5"/>
-        <v>2.8459200000000004</v>
-      </c>
-      <c r="L8">
-        <f>100-J8</f>
-        <v>95.934399999999997</v>
-      </c>
-      <c r="M8">
-        <f>100</f>
-        <v>100</v>
-      </c>
-      <c r="N8">
+        <v>196.97543999999999</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="6"/>
-        <v>295.93439999999998</v>
-      </c>
-      <c r="O8">
+        <v>100</v>
+      </c>
+      <c r="R8">
         <f t="shared" si="7"/>
-        <v>197.15407999999999</v>
-      </c>
-      <c r="P8">
+        <v>300</v>
+      </c>
+      <c r="S8">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="Q8">
+      <c r="T8">
         <f t="shared" si="9"/>
-        <v>300</v>
-      </c>
-      <c r="R8">
+        <v>892.65463999999997</v>
+      </c>
+      <c r="U8">
+        <f>500-100-J8</f>
+        <v>382.71679999999998</v>
+      </c>
+      <c r="V8">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="11"/>
-        <v>893.08848</v>
-      </c>
-      <c r="T8">
-        <f t="shared" si="12"/>
-        <v>383.73759999999999</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1140,81 +1173,85 @@
         <v>2800</v>
       </c>
       <c r="C9">
-        <v>25.8</v>
+        <v>32.6</v>
       </c>
       <c r="D9">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>1109.4000000000001</v>
+        <v>1304</v>
       </c>
       <c r="F9">
         <f>0.001*E9</f>
-        <v>1.1094000000000002</v>
+        <v>1.304</v>
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>44.376000000000005</v>
+        <v>52.16</v>
       </c>
       <c r="H9">
+        <f t="shared" si="3"/>
+        <v>12.159999999999997</v>
+      </c>
+      <c r="I9">
         <f>F9</f>
-        <v>1.1094000000000002</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="3"/>
-        <v>44.376000000000005</v>
+        <v>1.304</v>
       </c>
       <c r="J9">
+        <f>(I9*G9)/F9</f>
+        <v>52.16</v>
+      </c>
+      <c r="K9">
+        <f>I9*10</f>
+        <v>13.040000000000001</v>
+      </c>
+      <c r="L9">
+        <f>I9*7</f>
+        <v>9.1280000000000001</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:M12" si="11">100-K9</f>
+        <v>86.96</v>
+      </c>
+      <c r="N9">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="4"/>
-        <v>11.094000000000001</v>
-      </c>
-      <c r="K9">
+        <v>286.95999999999998</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="5"/>
-        <v>7.7658000000000014</v>
-      </c>
-      <c r="L9">
-        <f t="shared" ref="L9:L12" si="14">100-J9</f>
-        <v>88.906000000000006</v>
-      </c>
-      <c r="M9">
-        <f>100</f>
-        <v>100</v>
-      </c>
-      <c r="N9">
+        <v>190.87200000000001</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="6"/>
-        <v>288.90600000000001</v>
-      </c>
-      <c r="O9">
+        <v>100</v>
+      </c>
+      <c r="R9">
         <f t="shared" si="7"/>
-        <v>192.23419999999999</v>
-      </c>
-      <c r="P9">
+        <v>300</v>
+      </c>
+      <c r="S9">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="Q9">
+      <c r="T9">
         <f t="shared" si="9"/>
-        <v>300</v>
-      </c>
-      <c r="R9">
+        <v>877.83199999999999</v>
+      </c>
+      <c r="U9">
+        <f>500-100-J9</f>
+        <v>347.84000000000003</v>
+      </c>
+      <c r="V9">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="11"/>
-        <v>881.14020000000005</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="12"/>
-        <v>355.62400000000002</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1222,80 +1259,84 @@
         <v>500</v>
       </c>
       <c r="C10">
-        <v>163</v>
+        <v>1100</v>
       </c>
       <c r="D10">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>7172</v>
+        <v>44000</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>7.1719999999999997</v>
+        <v>44</v>
       </c>
       <c r="G10">
-        <f>(G17*G16)/25</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1760</v>
       </c>
       <c r="H10">
+        <f t="shared" si="3"/>
+        <v>1720</v>
+      </c>
+      <c r="I10">
         <v>4</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="J10">
+        <f>(I10*G10)/F10</f>
+        <v>160</v>
+      </c>
+      <c r="K10">
+        <f>I10*10</f>
+        <v>40</v>
+      </c>
+      <c r="L10">
+        <f>I10*7</f>
+        <v>28</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
+      <c r="N10">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="K10">
+        <v>260</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="5"/>
-        <v>28</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="14"/>
-        <v>60</v>
-      </c>
-      <c r="M10">
-        <f>100</f>
-        <v>100</v>
-      </c>
-      <c r="N10">
+        <v>172</v>
+      </c>
+      <c r="Q10">
         <f t="shared" si="6"/>
-        <v>260</v>
-      </c>
-      <c r="O10">
+        <v>100</v>
+      </c>
+      <c r="R10">
         <f t="shared" si="7"/>
-        <v>172</v>
-      </c>
-      <c r="P10">
+        <v>300</v>
+      </c>
+      <c r="S10">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="Q10">
+      <c r="T10">
         <f t="shared" si="9"/>
-        <v>300</v>
-      </c>
-      <c r="R10">
+        <v>832</v>
+      </c>
+      <c r="U10">
+        <f>500-100-J10</f>
+        <v>240</v>
+      </c>
+      <c r="V10">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="11"/>
-        <v>832</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="12"/>
-        <v>400</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1303,81 +1344,85 @@
         <v>2800</v>
       </c>
       <c r="C11">
-        <v>55.6</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="D11">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>2446.4</v>
+        <v>2896</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>2.4464000000000001</v>
+        <v>2.8959999999999999</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>97.856000000000009</v>
+        <v>115.84</v>
       </c>
       <c r="H11">
+        <f t="shared" si="3"/>
+        <v>75.84</v>
+      </c>
+      <c r="I11">
         <f>F11</f>
-        <v>2.4464000000000001</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="3"/>
-        <v>97.856000000000009</v>
+        <v>2.8959999999999999</v>
       </c>
       <c r="J11">
+        <f>(I11*G11)/F11</f>
+        <v>115.84</v>
+      </c>
+      <c r="K11">
+        <f>I11*10</f>
+        <v>28.96</v>
+      </c>
+      <c r="L11">
+        <f>I11*7</f>
+        <v>20.271999999999998</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="11"/>
+        <v>71.039999999999992</v>
+      </c>
+      <c r="N11">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="O11">
         <f t="shared" si="4"/>
-        <v>24.464000000000002</v>
-      </c>
-      <c r="K11">
+        <v>271.03999999999996</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="5"/>
-        <v>17.1248</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="14"/>
-        <v>75.536000000000001</v>
-      </c>
-      <c r="M11">
-        <f>100</f>
-        <v>100</v>
-      </c>
-      <c r="N11">
+        <v>179.72800000000001</v>
+      </c>
+      <c r="Q11">
         <f t="shared" si="6"/>
-        <v>275.536</v>
-      </c>
-      <c r="O11">
+        <v>100</v>
+      </c>
+      <c r="R11">
         <f t="shared" si="7"/>
-        <v>182.87520000000001</v>
-      </c>
-      <c r="P11">
+        <v>300</v>
+      </c>
+      <c r="S11">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="Q11">
+      <c r="T11">
         <f t="shared" si="9"/>
-        <v>300</v>
-      </c>
-      <c r="R11">
+        <v>850.76800000000003</v>
+      </c>
+      <c r="U11">
+        <f>500-100-J11</f>
+        <v>284.15999999999997</v>
+      </c>
+      <c r="V11">
         <f t="shared" si="10"/>
-        <v>100</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="11"/>
-        <v>858.41120000000001</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="12"/>
-        <v>302.14400000000001</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="13"/>
         <v>800</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1385,118 +1430,123 @@
         <v>2800</v>
       </c>
       <c r="C12">
-        <v>99.4</v>
+        <v>60.8</v>
       </c>
       <c r="D12">
         <v>44</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>4373.6000000000004</v>
+        <v>2675.2</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>4.3736000000000006</v>
+        <v>2.6751999999999998</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>174.94400000000002</v>
+        <v>107.008</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>63.007999999999996</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
-        <v>160</v>
+        <f>F12</f>
+        <v>2.6751999999999998</v>
       </c>
       <c r="J12">
+        <f>(I12*G12)/F12</f>
+        <v>107.008</v>
+      </c>
+      <c r="K12">
+        <f>I12*10</f>
+        <v>26.751999999999999</v>
+      </c>
+      <c r="L12">
+        <f>I12*7</f>
+        <v>18.726399999999998</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="11"/>
+        <v>73.248000000000005</v>
+      </c>
+      <c r="N12">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="O12">
         <f t="shared" si="4"/>
-        <v>40</v>
-      </c>
-      <c r="K12">
+        <v>273.24799999999999</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="5"/>
-        <v>28</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="14"/>
-        <v>60</v>
-      </c>
-      <c r="M12">
-        <f>100</f>
-        <v>100</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="6"/>
-        <v>260</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="7"/>
-        <v>172</v>
-      </c>
-      <c r="P12">
-        <f t="shared" ref="P12" si="15">M12</f>
-        <v>100</v>
+        <v>181.27359999999999</v>
       </c>
       <c r="Q12">
-        <f t="shared" ref="Q12" si="16">3*P12</f>
+        <f t="shared" ref="Q12" si="12">N12</f>
+        <v>100</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ref="R12" si="13">3*Q12</f>
         <v>300</v>
       </c>
-      <c r="R12">
-        <f t="shared" ref="R12" si="17">P12</f>
-        <v>100</v>
-      </c>
       <c r="S12">
-        <f t="shared" si="11"/>
-        <v>832</v>
+        <f t="shared" ref="S12" si="14">Q12</f>
+        <v>100</v>
       </c>
       <c r="T12">
-        <f t="shared" si="12"/>
-        <v>240</v>
+        <f t="shared" si="9"/>
+        <v>854.52160000000003</v>
       </c>
       <c r="U12">
-        <f t="shared" si="13"/>
+        <f>500-100-J12</f>
+        <v>292.99200000000002</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="10"/>
         <v>800</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:22">
       <c r="A13" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="J13">
-        <f>SUM(J2:J12)</f>
-        <v>340.03960000000001</v>
-      </c>
       <c r="K13">
         <f>SUM(K2:K12)</f>
-        <v>238.02772000000002</v>
-      </c>
-      <c r="S13">
-        <f>SUM(S2:S12)</f>
-        <v>9182.348680000001</v>
-      </c>
-      <c r="U13">
-        <f>SUM(U2:U12)</f>
+        <v>353.07279999999997</v>
+      </c>
+      <c r="L13">
+        <f>SUM(L2:L12)</f>
+        <v>247.15096</v>
+      </c>
+      <c r="T13">
+        <f>SUM(T2:T12)</f>
+        <v>9179.7762399999992</v>
+      </c>
+      <c r="V13">
+        <f>SUM(V2:V12)</f>
         <v>8800</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
-      <c r="S14">
-        <f>S13*0.001</f>
-        <v>9.1823486800000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
-      <c r="U15">
-        <f>SUM(U13,S13)</f>
-        <v>17982.348680000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+    <row r="14" spans="1:22">
+      <c r="T14">
+        <f>T13*0.001</f>
+        <v>9.1797762399999989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="V15">
+        <f>SUM(V13,T13)</f>
+        <v>17979.776239999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="F16" s="3"/>
-      <c r="U16">
-        <f>U15/1000</f>
-        <v>17.982348680000001</v>
+      <c r="V16">
+        <f>V15/1000</f>
+        <v>17.97977624</v>
       </c>
     </row>
     <row r="17" spans="6:6">
@@ -1510,7 +1560,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="94" fitToWidth="2" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="L4 L7 G10" formula="1"/>
+    <ignoredError sqref="M4 M7" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>